<commit_message>
loading second BSSs in from KwaZulu-Natal & Free State
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="114">
   <si>
     <t>WEALTH GROUP</t>
   </si>
@@ -434,11 +434,17 @@
   <si>
     <t>Other Items</t>
   </si>
+  <si>
+    <t>Factor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -692,7 +698,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -779,6 +785,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="72">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1280,10 +1290,10 @@
   </sheetPr>
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="F31" sqref="F31"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1307,8 +1317,13 @@
       <c r="D1" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="E1" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="53">
+        <f>IF(UPPER(D1)="KJ",4.1868,IF(OR(UPPER(D1)="KCAL",AND(CODE(LEFT(D1))=67,UPPER(MID(D1,2,LEN(D1)-1))="AL")),1,IF(AND(CODE(LEFT(D1))=99,UPPER(MID(D1,2,LEN(D1)-1))="AL"),1000,0)))</f>
+        <v>4.1867999999999999</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="14" thickBot="1">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
Corrected expandability of cattle for VP -- DONE
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -1288,12 +1288,12 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2032,7 +2032,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13">
+    <row r="49" spans="1:10" ht="13">
       <c r="A49" s="43" t="s">
         <v>80</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13">
+    <row r="50" spans="1:10" ht="13">
       <c r="A50" s="44" t="s">
         <v>81</v>
       </c>
@@ -2077,8 +2077,12 @@
       <c r="I50" s="18" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="13">
+      <c r="J50" s="19">
+        <f>G50*H50</f>
+        <v>401.29673907782717</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="13">
       <c r="A51" s="43" t="s">
         <v>82</v>
       </c>
@@ -2101,7 +2105,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13">
+    <row r="52" spans="1:10" ht="13">
       <c r="A52" s="43" t="s">
         <v>85</v>
       </c>
@@ -2124,7 +2128,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13">
+    <row r="53" spans="1:10" ht="13">
       <c r="A53" s="43" t="s">
         <v>29</v>
       </c>
@@ -2147,7 +2151,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="13">
+    <row r="54" spans="1:10" ht="13">
       <c r="A54" s="43" t="s">
         <v>87</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13">
+    <row r="55" spans="1:10" ht="13">
       <c r="A55" s="43" t="s">
         <v>88</v>
       </c>
@@ -2193,7 +2197,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="13">
+    <row r="56" spans="1:10" ht="13">
       <c r="A56" s="43" t="s">
         <v>89</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="13">
+    <row r="57" spans="1:10" ht="13">
       <c r="A57" s="43" t="s">
         <v>90</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13">
+    <row r="58" spans="1:10" ht="13">
       <c r="A58" s="43" t="s">
         <v>92</v>
       </c>
@@ -2262,7 +2266,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="13">
+    <row r="59" spans="1:10" ht="13">
       <c r="A59" s="43" t="s">
         <v>93</v>
       </c>
@@ -2285,7 +2289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13">
+    <row r="60" spans="1:10" ht="13">
       <c r="A60" s="43" t="s">
         <v>94</v>
       </c>
@@ -2308,7 +2312,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="13">
+    <row r="61" spans="1:10" ht="13">
       <c r="A61" s="43" t="s">
         <v>83</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="13">
+    <row r="62" spans="1:10" ht="13">
       <c r="A62" s="43" t="s">
         <v>84</v>
       </c>
@@ -2354,7 +2358,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="13">
+    <row r="63" spans="1:10" ht="13">
       <c r="A63" s="43" t="s">
         <v>95</v>
       </c>
@@ -2377,7 +2381,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="13">
+    <row r="64" spans="1:10" ht="13">
       <c r="A64" s="43" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
All zones: switched on protection and saved --DONE
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -1288,12 +1288,12 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="J50" sqref="J50"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="24">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="D14" s="24">
         <v>0.33</v>
@@ -2032,7 +2032,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="13">
+    <row r="49" spans="1:9" ht="13">
       <c r="A49" s="43" t="s">
         <v>80</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="13">
+    <row r="50" spans="1:9" ht="13">
       <c r="A50" s="44" t="s">
         <v>81</v>
       </c>
@@ -2077,12 +2077,8 @@
       <c r="I50" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J50" s="19">
-        <f>G50*H50</f>
-        <v>401.29673907782717</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="13">
+    </row>
+    <row r="51" spans="1:9" ht="13">
       <c r="A51" s="43" t="s">
         <v>82</v>
       </c>
@@ -2105,7 +2101,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="13">
+    <row r="52" spans="1:9" ht="13">
       <c r="A52" s="43" t="s">
         <v>85</v>
       </c>
@@ -2128,7 +2124,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="13">
+    <row r="53" spans="1:9" ht="13">
       <c r="A53" s="43" t="s">
         <v>29</v>
       </c>
@@ -2151,7 +2147,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="13">
+    <row r="54" spans="1:9" ht="13">
       <c r="A54" s="43" t="s">
         <v>87</v>
       </c>
@@ -2174,7 +2170,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="13">
+    <row r="55" spans="1:9" ht="13">
       <c r="A55" s="43" t="s">
         <v>88</v>
       </c>
@@ -2197,7 +2193,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="13">
+    <row r="56" spans="1:9" ht="13">
       <c r="A56" s="43" t="s">
         <v>89</v>
       </c>
@@ -2220,7 +2216,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="13">
+    <row r="57" spans="1:9" ht="13">
       <c r="A57" s="43" t="s">
         <v>90</v>
       </c>
@@ -2243,7 +2239,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="13">
+    <row r="58" spans="1:9" ht="13">
       <c r="A58" s="43" t="s">
         <v>92</v>
       </c>
@@ -2266,7 +2262,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="13">
+    <row r="59" spans="1:9" ht="13">
       <c r="A59" s="43" t="s">
         <v>93</v>
       </c>
@@ -2289,7 +2285,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="13">
+    <row r="60" spans="1:9" ht="13">
       <c r="A60" s="43" t="s">
         <v>94</v>
       </c>
@@ -2312,7 +2308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="13">
+    <row r="61" spans="1:9" ht="13">
       <c r="A61" s="43" t="s">
         <v>83</v>
       </c>
@@ -2335,7 +2331,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="13">
+    <row r="62" spans="1:9" ht="13">
       <c r="A62" s="43" t="s">
         <v>84</v>
       </c>
@@ -2358,7 +2354,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="13">
+    <row r="63" spans="1:9" ht="13">
       <c r="A63" s="43" t="s">
         <v>95</v>
       </c>
@@ -2381,7 +2377,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="13">
+    <row r="64" spans="1:9" ht="13">
       <c r="A64" s="43" t="s">
         <v>96</v>
       </c>
@@ -3402,6 +3398,7 @@
       <c r="G108" s="19"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="7">
     <mergeCell ref="C92:F92"/>
     <mergeCell ref="C95:F95"/>

</xml_diff>

<commit_message>
Changed the staple purchase maize only from 'yes' to 'no'
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -315,9 +315,6 @@
     <t>Addition</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>wheat</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1293,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+      <selection pane="topRight" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1309,16 +1309,16 @@
     <row r="1" spans="1:6" ht="13">
       <c r="A1" s="45"/>
       <c r="B1" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="18">
         <v>8800</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="50">
         <f>IF(UPPER(D1)="KJ",4.1868,IF(OR(UPPER(D1)="KCAL",AND(CODE(LEFT(D1))=67,UPPER(MID(D1,2,LEN(D1)-1))="AL")),1,IF(AND(CODE(LEFT(D1))=99,UPPER(MID(D1,2,LEN(D1)-1))="AL"),1000,0)))</f>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="23" spans="1:6" ht="13">
       <c r="A23" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="24">
@@ -1627,7 +1627,7 @@
     </row>
     <row r="24" spans="1:6" ht="13">
       <c r="A24" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="24">
@@ -1866,7 +1866,7 @@
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
       <c r="D41" s="24" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
@@ -1876,7 +1876,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>71</v>
@@ -1885,10 +1885,10 @@
       <c r="E42" s="52"/>
       <c r="F42" s="53"/>
       <c r="G42" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="46" t="s">
         <v>100</v>
-      </c>
-      <c r="H42" s="46" t="s">
-        <v>101</v>
       </c>
       <c r="I42" s="18" t="s">
         <v>59</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="43" spans="1:9" ht="13">
       <c r="A43" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="24">
@@ -1914,15 +1914,15 @@
         <v>13.123144876325089</v>
       </c>
       <c r="I43" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="13">
       <c r="A44" s="43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="24">
@@ -1937,15 +1937,15 @@
         <v>8.8394160583941606</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="13">
       <c r="A45" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="24">
@@ -1960,15 +1960,15 @@
         <v>21.973882175226581</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13">
       <c r="A46" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" s="31"/>
       <c r="D46" s="24">
@@ -1983,15 +1983,15 @@
         <v>31.553656697662728</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="13">
       <c r="A47" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="24">
@@ -2006,15 +2006,15 @@
         <v>61.072224244630505</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="13">
       <c r="A48" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="24">
@@ -2029,15 +2029,15 @@
         <v>46.997666110978805</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="13">
       <c r="A49" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="24">
@@ -2052,15 +2052,15 @@
         <v>41.423255813953475</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="13">
       <c r="A50" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="41">
@@ -2075,15 +2075,15 @@
         <v>8.3410435001004615</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="13">
       <c r="A51" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="24">
@@ -2098,15 +2098,15 @@
         <v>9.5639402715495763</v>
       </c>
       <c r="I51" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="13">
       <c r="A52" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="24">
@@ -2121,7 +2121,7 @@
         <v>13.024845827540727</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="13">
@@ -2129,7 +2129,7 @@
         <v>29</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="24">
@@ -2144,15 +2144,15 @@
         <v>18.190370196813497</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="13">
       <c r="A54" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="24">
@@ -2167,15 +2167,15 @@
         <v>8.3023255813953476</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13">
       <c r="A55" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="24">
@@ -2190,15 +2190,15 @@
         <v>13.548061389337644</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="13">
       <c r="A56" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="24">
@@ -2213,15 +2213,15 @@
         <v>8.5805747126436778</v>
       </c>
       <c r="I56" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="13">
       <c r="A57" s="43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="24">
@@ -2236,15 +2236,15 @@
         <v>5.9211901121304793</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13">
       <c r="A58" s="43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="24">
@@ -2259,15 +2259,15 @@
         <v>8.9993857493857483</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="13">
       <c r="A59" s="43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="31"/>
       <c r="D59" s="24">
@@ -2282,15 +2282,15 @@
         <v>58.337174721189591</v>
       </c>
       <c r="I59" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="13">
       <c r="A60" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="24">
@@ -2305,15 +2305,15 @@
         <v>86.204819277108442</v>
       </c>
       <c r="I60" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="13">
       <c r="A61" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="24">
@@ -2328,15 +2328,15 @@
         <v>21.820450281425892</v>
       </c>
       <c r="I61" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="13">
       <c r="A62" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="24">
@@ -2351,15 +2351,15 @@
         <v>22.545391356905412</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="13">
       <c r="A63" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="24">
@@ -2374,15 +2374,15 @@
         <v>49.094871794871793</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="13">
       <c r="A64" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="24">
@@ -2397,15 +2397,15 @@
         <v>31.162500000000001</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="13">
       <c r="A65" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="24">
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="13">
@@ -2428,7 +2428,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="24">
@@ -2443,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="13">
@@ -2451,7 +2451,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="24">
@@ -2466,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="13">
@@ -2474,7 +2474,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="24">
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="13">
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="13">
@@ -2520,7 +2520,7 @@
         <v>32</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C70" s="51" t="s">
         <v>71</v>
@@ -2532,7 +2532,7 @@
         <v>72</v>
       </c>
       <c r="H70" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="13">
@@ -2540,7 +2540,7 @@
         <v>33</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" s="24">
         <v>1</v>
@@ -2558,7 +2558,7 @@
         <v>40</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="13">
@@ -2566,7 +2566,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72" s="24">
         <v>0.75</v>
@@ -2584,7 +2584,7 @@
         <v>15</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="13">
@@ -2592,7 +2592,7 @@
         <v>35</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="24">
         <f>260/420</f>
@@ -2614,7 +2614,7 @@
         <v>100</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="13">
@@ -2622,7 +2622,7 @@
         <v>36</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C74" s="24">
         <v>0.5</v>
@@ -2640,7 +2640,7 @@
         <v>100</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="13">
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="13">
@@ -2674,7 +2674,7 @@
         <v>38</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="24">
         <v>1</v>
@@ -2692,7 +2692,7 @@
         <v>200</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="13">
@@ -2718,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="13">
@@ -2726,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C78" s="24">
         <v>1</v>
@@ -2745,7 +2745,7 @@
         <v>300</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="13">
@@ -2753,7 +2753,7 @@
         <v>64</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="24">
         <v>1</v>
@@ -2773,7 +2773,7 @@
         <v>88</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13">
@@ -2781,7 +2781,7 @@
         <v>69</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="24">
         <v>1</v>
@@ -2799,7 +2799,7 @@
         <v>60</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13">
@@ -2825,7 +2825,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="13">
@@ -2833,7 +2833,7 @@
         <v>65</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="24">
@@ -2845,12 +2845,12 @@
         <v>7.5</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="13">
       <c r="A83" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B83" s="33"/>
       <c r="C83" s="51" t="s">
@@ -2863,15 +2863,15 @@
         <v>72</v>
       </c>
       <c r="H83" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="13">
       <c r="A84" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="31"/>
       <c r="D84" s="24">
@@ -2887,15 +2887,15 @@
         <v>1</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="13">
       <c r="A85" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C85" s="31"/>
       <c r="D85" s="24">
@@ -2911,12 +2911,12 @@
         <v>1</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="13">
       <c r="A86" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="33"/>
       <c r="C86" s="51" t="s">
@@ -2929,7 +2929,7 @@
         <v>72</v>
       </c>
       <c r="H86" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="13">
@@ -2955,7 +2955,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="13">
@@ -2963,7 +2963,7 @@
         <v>31</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C88" s="31"/>
       <c r="D88" s="24">
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13">
@@ -2993,7 +2993,7 @@
         <v>72</v>
       </c>
       <c r="H89" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="13">
@@ -3001,7 +3001,7 @@
         <v>41</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90" s="31"/>
       <c r="D90" s="24">
@@ -3014,7 +3014,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="I90" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="13">
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="13">
@@ -3058,7 +3058,7 @@
         <v>72</v>
       </c>
       <c r="H92" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="13">
@@ -3066,7 +3066,7 @@
         <v>44</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93" s="24">
         <v>1</v>
@@ -3087,7 +3087,7 @@
         <v>150</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="13">
@@ -3095,7 +3095,7 @@
         <v>45</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94" s="31"/>
       <c r="D94" s="24">
@@ -3107,7 +3107,7 @@
         <v>70</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="13">
@@ -3125,7 +3125,7 @@
         <v>72</v>
       </c>
       <c r="H95" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="13">
@@ -3151,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="13">
@@ -3177,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="I97" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="13">
@@ -3203,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="I98" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="13">
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="I99" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="13">
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="I100" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="13">
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="I101" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="13">
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="I102" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="13">
@@ -3333,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="I103" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="13">
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="I104" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="13">
@@ -3385,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="I105" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:9">

</xml_diff>

<commit_message>
Added in Limpopo/Mpumalanga BSSs, updated others
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ExpFactors" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <definedName name="WGI_data">#REF!</definedName>
     <definedName name="WGI_WB">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -934,6 +934,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1296,17 +1301,17 @@
       <selection pane="topRight" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="19" customWidth="1"/>
-    <col min="3" max="6" width="6.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="19"/>
+    <col min="1" max="1" width="20.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="19" customWidth="1"/>
+    <col min="3" max="6" width="6.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="45" t="s">
         <v>96</v>
@@ -1325,7 +1330,7 @@
         <v>4.1867999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +1340,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="14" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1345,7 +1350,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="13">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1373,7 +1378,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="13">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1388,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:6" ht="13">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1398,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="13">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1421,7 +1426,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="13">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
@@ -1431,7 +1436,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="13">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1454,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13">
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1467,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1482,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="13">
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13">
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1513,7 +1518,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1523,7 +1528,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="13">
+    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1559,7 +1564,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1574,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="13">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
@@ -1579,7 +1584,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>58</v>
       </c>
@@ -1597,7 +1602,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>57</v>
       </c>
@@ -1607,7 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="13">
+    <row r="23" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>74</v>
       </c>
@@ -1625,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13">
+    <row r="24" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>73</v>
       </c>
@@ -1643,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13">
+    <row r="25" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1666,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>20</v>
       </c>
@@ -1671,7 +1676,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="13">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
@@ -1681,7 +1686,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="13">
+    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>23</v>
       </c>
@@ -1709,7 +1714,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="13">
+    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
@@ -1727,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1742,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="13">
+    <row r="32" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
@@ -1755,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +1770,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="13">
+    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>22</v>
       </c>
@@ -1783,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="13">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1793,7 +1798,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="13">
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="13">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>27</v>
       </c>
@@ -1821,7 +1826,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="13">
+    <row r="38" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="13">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>9</v>
       </c>
@@ -1849,7 +1854,7 @@
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
     </row>
-    <row r="40" spans="1:9" ht="13">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>61</v>
       </c>
@@ -1859,7 +1864,7 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
     </row>
-    <row r="41" spans="1:9" ht="13">
+    <row r="41" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
@@ -1871,7 +1876,7 @@
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="13">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>28</v>
       </c>
@@ -1894,7 +1899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="13">
+    <row r="43" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="43" t="s">
         <v>75</v>
       </c>
@@ -1917,7 +1922,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="13">
+    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="43" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1945,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="13">
+    <row r="45" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="43" t="s">
         <v>85</v>
       </c>
@@ -1963,7 +1968,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="13">
+    <row r="46" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="43" t="s">
         <v>77</v>
       </c>
@@ -1986,7 +1991,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="13">
+    <row r="47" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="43" t="s">
         <v>104</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="13">
+    <row r="48" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
         <v>78</v>
       </c>
@@ -2032,7 +2037,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13">
+    <row r="49" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="43" t="s">
         <v>79</v>
       </c>
@@ -2055,7 +2060,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13">
+    <row r="50" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
         <v>80</v>
       </c>
@@ -2078,7 +2083,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13">
+    <row r="51" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="43" t="s">
         <v>81</v>
       </c>
@@ -2101,7 +2106,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13">
+    <row r="52" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="43" t="s">
         <v>84</v>
       </c>
@@ -2124,7 +2129,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13">
+    <row r="53" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="43" t="s">
         <v>29</v>
       </c>
@@ -2147,7 +2152,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="13">
+    <row r="54" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="43" t="s">
         <v>86</v>
       </c>
@@ -2170,7 +2175,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13">
+    <row r="55" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="43" t="s">
         <v>87</v>
       </c>
@@ -2193,7 +2198,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="13">
+    <row r="56" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="43" t="s">
         <v>88</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="13">
+    <row r="57" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="43" t="s">
         <v>89</v>
       </c>
@@ -2239,7 +2244,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13">
+    <row r="58" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="43" t="s">
         <v>91</v>
       </c>
@@ -2262,7 +2267,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="13">
+    <row r="59" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="43" t="s">
         <v>92</v>
       </c>
@@ -2285,7 +2290,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13">
+    <row r="60" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="43" t="s">
         <v>93</v>
       </c>
@@ -2308,7 +2313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="13">
+    <row r="61" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="43" t="s">
         <v>82</v>
       </c>
@@ -2331,7 +2336,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="13">
+    <row r="62" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="43" t="s">
         <v>83</v>
       </c>
@@ -2354,7 +2359,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="13">
+    <row r="63" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="43" t="s">
         <v>94</v>
       </c>
@@ -2377,7 +2382,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="13">
+    <row r="64" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="43" t="s">
         <v>95</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="13">
+    <row r="65" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>90</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="13">
+    <row r="66" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>66</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13">
+    <row r="67" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>67</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="13">
+    <row r="68" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -2492,7 +2497,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13">
+    <row r="69" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>31</v>
       </c>
@@ -2515,7 +2520,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="13">
+    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>32</v>
       </c>
@@ -2535,7 +2540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="13">
+    <row r="71" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="34" t="s">
         <v>33</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13">
+    <row r="72" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="34" t="s">
         <v>34</v>
       </c>
@@ -2587,7 +2592,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13">
+    <row r="73" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="34" t="s">
         <v>35</v>
       </c>
@@ -2617,7 +2622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13">
+    <row r="74" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="34" t="s">
         <v>36</v>
       </c>
@@ -2643,7 +2648,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13">
+    <row r="75" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="34" t="s">
         <v>37</v>
       </c>
@@ -2669,7 +2674,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13">
+    <row r="76" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="34" t="s">
         <v>38</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13">
+    <row r="77" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="34" t="s">
         <v>39</v>
       </c>
@@ -2721,7 +2726,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="13">
+    <row r="78" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A78" s="34" t="s">
         <v>2</v>
       </c>
@@ -2748,7 +2753,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="13">
+    <row r="79" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A79" s="34" t="s">
         <v>64</v>
       </c>
@@ -2776,7 +2781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="13">
+    <row r="80" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="34" t="s">
         <v>69</v>
       </c>
@@ -2802,7 +2807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="13">
+    <row r="81" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A81" s="34" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2833,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="13">
+    <row r="82" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>65</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="13">
+    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="32" t="s">
         <v>107</v>
       </c>
@@ -2866,7 +2871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="13">
+    <row r="84" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="34" t="s">
         <v>109</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="13">
+    <row r="85" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A85" s="34" t="s">
         <v>110</v>
       </c>
@@ -2914,7 +2919,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="13">
+    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="32" t="s">
         <v>111</v>
       </c>
@@ -2932,7 +2937,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="13">
+    <row r="87" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>70</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="13">
+    <row r="88" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>31</v>
       </c>
@@ -2978,7 +2983,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="13">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="32" t="s">
         <v>40</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="13">
+    <row r="90" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
         <v>41</v>
       </c>
@@ -3017,7 +3022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="13">
+    <row r="91" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>42</v>
       </c>
@@ -3043,7 +3048,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="13">
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
         <v>43</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="13">
+    <row r="93" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A93" s="34" t="s">
         <v>44</v>
       </c>
@@ -3090,7 +3095,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="13">
+    <row r="94" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A94" s="34" t="s">
         <v>45</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13">
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="32" t="s">
         <v>46</v>
       </c>
@@ -3128,7 +3133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="13">
+    <row r="96" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A96" s="34" t="s">
         <v>47</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="13">
+    <row r="97" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>48</v>
       </c>
@@ -3180,7 +3185,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="13">
+    <row r="98" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A98" s="34" t="s">
         <v>49</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="13">
+    <row r="99" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A99" s="34" t="s">
         <v>50</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="13">
+    <row r="100" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
         <v>51</v>
       </c>
@@ -3258,7 +3263,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="13">
+    <row r="101" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="34" t="s">
         <v>52</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="13">
+    <row r="102" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="34" t="s">
         <v>53</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="13">
+    <row r="103" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="34" t="s">
         <v>54</v>
       </c>
@@ -3336,7 +3341,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="13">
+    <row r="104" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>55</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="13">
+    <row r="105" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
         <v>56</v>
       </c>
@@ -3388,13 +3393,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G106" s="19"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G107" s="19"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G108" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected error in za_expandabilityfactors.xlsx, as well as others
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="ExpFactors" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <definedName name="WGI_data">#REF!</definedName>
     <definedName name="WGI_WB">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
   <si>
     <t>WEALTH GROUP</t>
   </si>
@@ -315,6 +315,9 @@
     <t>Addition</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>wheat</t>
   </si>
   <si>
@@ -430,20 +433,15 @@
   </si>
   <si>
     <t>Other Items</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -624,7 +622,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -697,8 +695,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -776,10 +777,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="72" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,8 +788,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="75">
+    <cellStyle name="Comma" xfId="72" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -826,6 +827,7 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -861,6 +863,7 @@
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -934,11 +937,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1293,44 +1291,43 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="D41" sqref="D41"/>
+      <selection pane="topRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="19" customWidth="1"/>
-    <col min="3" max="6" width="6.42578125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="20.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="19" customWidth="1"/>
+    <col min="3" max="6" width="6.5" style="19" customWidth="1"/>
+    <col min="7" max="7" width="27" style="35" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="19" customWidth="1"/>
+    <col min="9" max="11" width="9.1640625" style="19"/>
+    <col min="12" max="12" width="9.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13">
       <c r="A1" s="45"/>
       <c r="B1" s="45" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" s="18">
         <v>8800</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="50">
-        <f>IF(UPPER(D1)="KJ",4.1868,IF(OR(UPPER(D1)="KCAL",AND(CODE(LEFT(D1))=67,UPPER(MID(D1,2,LEN(D1)-1))="AL")),1,IF(AND(CODE(LEFT(D1))=99,UPPER(MID(D1,2,LEN(D1)-1))="AL"),1000,0)))</f>
+        <v>98</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="54">
         <v>4.1867999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1340,7 +1337,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14" thickBot="1">
       <c r="A3" s="21"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1350,7 +1347,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="13">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1378,7 +1375,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1388,7 +1385,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1398,7 +1395,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1413,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1426,7 +1423,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13">
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
@@ -1436,7 +1433,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1454,7 +1451,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="13">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1472,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
@@ -1482,13 +1479,13 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="13">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="24">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="D14" s="24">
         <v>0.33</v>
@@ -1500,7 +1497,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="13">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="13">
       <c r="A16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1528,7 +1525,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="13">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1546,7 +1543,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1564,7 +1561,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1571,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13">
       <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
@@ -1584,7 +1581,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="13">
       <c r="A21" s="8" t="s">
         <v>58</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13">
       <c r="A22" s="11" t="s">
         <v>57</v>
       </c>
@@ -1612,9 +1609,9 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="13">
       <c r="A23" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="24">
@@ -1630,9 +1627,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="13">
       <c r="A24" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="24">
@@ -1648,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="13">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13">
       <c r="A26" s="10" t="s">
         <v>20</v>
       </c>
@@ -1676,7 +1673,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
@@ -1686,7 +1683,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="13">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13">
       <c r="A29" s="11" t="s">
         <v>23</v>
       </c>
@@ -1714,7 +1711,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="13">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
@@ -1732,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13">
       <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1739,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="13">
       <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
@@ -1760,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="13">
       <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
@@ -1770,7 +1767,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="13">
       <c r="A34" s="8" t="s">
         <v>22</v>
       </c>
@@ -1788,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="13">
       <c r="A35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1798,7 +1795,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="13">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -1816,7 +1813,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="13">
       <c r="A37" s="11" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1823,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="13">
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
@@ -1844,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="13">
       <c r="A39" s="15" t="s">
         <v>9</v>
       </c>
@@ -1854,7 +1851,7 @@
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="13">
       <c r="A40" s="27" t="s">
         <v>61</v>
       </c>
@@ -1864,24 +1861,24 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
     </row>
-    <row r="41" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="13">
       <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
       <c r="D41" s="24" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="13">
       <c r="A42" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>71</v>
@@ -1890,21 +1887,21 @@
       <c r="E42" s="52"/>
       <c r="F42" s="53"/>
       <c r="G42" s="46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H42" s="46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I42" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="13">
       <c r="A43" s="43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="24">
@@ -1919,15 +1916,22 @@
         <v>13.123144876325089</v>
       </c>
       <c r="I43" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K43" s="19">
+        <v>1800</v>
+      </c>
+      <c r="L43" s="49">
+        <f>G43*K43/365</f>
+        <v>74.454730635501633</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13">
       <c r="A44" s="43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C44" s="31"/>
       <c r="D44" s="24">
@@ -1942,15 +1946,22 @@
         <v>8.8394160583941606</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K44" s="19">
+        <v>2680</v>
+      </c>
+      <c r="L44" s="49">
+        <f t="shared" ref="L44:L69" si="0">G44*K44/365</f>
+        <v>36.846276167116933</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="13">
       <c r="A45" s="43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C45" s="31"/>
       <c r="D45" s="24">
@@ -1965,15 +1976,22 @@
         <v>21.973882175226581</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K45" s="19">
+        <v>6615</v>
+      </c>
+      <c r="L45" s="49">
+        <f t="shared" si="0"/>
+        <v>58.531874061110436</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="13">
       <c r="A46" s="43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C46" s="31"/>
       <c r="D46" s="24">
@@ -1988,15 +2006,22 @@
         <v>31.553656697662728</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K46" s="19">
+        <v>8980</v>
+      </c>
+      <c r="L46" s="49">
+        <f t="shared" si="0"/>
+        <v>572.70207150558451</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="13">
       <c r="A47" s="43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="24">
@@ -2011,15 +2036,22 @@
         <v>61.072224244630505</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K47" s="19">
+        <v>9840</v>
+      </c>
+      <c r="L47" s="49">
+        <f t="shared" si="0"/>
+        <v>92.276493816893989</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="13">
       <c r="A48" s="43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="24">
@@ -2034,15 +2066,22 @@
         <v>46.997666110978805</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K48" s="19">
+        <v>11760</v>
+      </c>
+      <c r="L48" s="49">
+        <f t="shared" si="0"/>
+        <v>41.488885600661646</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="13">
       <c r="A49" s="43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="31"/>
       <c r="D49" s="24">
@@ -2057,15 +2096,22 @@
         <v>41.423255813953475</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K49" s="19">
+        <v>4399</v>
+      </c>
+      <c r="L49" s="49">
+        <f t="shared" si="0"/>
+        <v>20.512302364940155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="13">
       <c r="A50" s="44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="41">
@@ -2080,15 +2126,22 @@
         <v>8.3410435001004615</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K50" s="19">
+        <v>10170</v>
+      </c>
+      <c r="L50" s="49">
+        <f t="shared" si="0"/>
+        <v>1340.5201085459428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="13">
       <c r="A51" s="43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="24">
@@ -2103,15 +2156,22 @@
         <v>9.5639402715495763</v>
       </c>
       <c r="I51" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K51" s="19">
+        <v>10060</v>
+      </c>
+      <c r="L51" s="49">
+        <f t="shared" si="0"/>
+        <v>315.90496832020824</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="13">
       <c r="A52" s="43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="24">
@@ -2126,15 +2186,22 @@
         <v>13.024845827540727</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K52" s="19">
+        <v>14820</v>
+      </c>
+      <c r="L52" s="49">
+        <f t="shared" si="0"/>
+        <v>367.31370647216102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="13">
       <c r="A53" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="24">
@@ -2149,15 +2216,22 @@
         <v>18.190370196813497</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K53" s="19">
+        <v>37680</v>
+      </c>
+      <c r="L53" s="49">
+        <f t="shared" si="0"/>
+        <v>609.14353013781579</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="13">
       <c r="A54" s="43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="24">
@@ -2172,15 +2246,22 @@
         <v>8.3023255813953476</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K54" s="19">
+        <v>3140</v>
+      </c>
+      <c r="L54" s="49">
+        <f t="shared" si="0"/>
+        <v>60.277860084347942</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="13">
       <c r="A55" s="43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="24">
@@ -2195,15 +2276,22 @@
         <v>13.548061389337644</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K55" s="19">
+        <v>840</v>
+      </c>
+      <c r="L55" s="49">
+        <f t="shared" si="0"/>
+        <v>10.509610259708465</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="13">
       <c r="A56" s="43" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="24">
@@ -2218,15 +2306,22 @@
         <v>8.5805747126436778</v>
       </c>
       <c r="I56" s="40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K56" s="19">
+        <v>2010</v>
+      </c>
+      <c r="L56" s="49">
+        <f t="shared" si="0"/>
+        <v>22.383511270210828</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="13">
       <c r="A57" s="43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="24">
@@ -2241,15 +2336,22 @@
         <v>5.9211901121304793</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K57" s="19">
+        <v>4860</v>
+      </c>
+      <c r="L57" s="49">
+        <f t="shared" si="0"/>
+        <v>56.756830312536998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="13">
       <c r="A58" s="43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="24">
@@ -2264,15 +2366,22 @@
         <v>8.9993857493857483</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K58" s="19">
+        <v>960</v>
+      </c>
+      <c r="L58" s="49">
+        <f t="shared" si="0"/>
+        <v>15.289724472633445</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="13">
       <c r="A59" s="43" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C59" s="31"/>
       <c r="D59" s="24">
@@ -2287,15 +2396,22 @@
         <v>58.337174721189591</v>
       </c>
       <c r="I59" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K59" s="19">
+        <v>11180</v>
+      </c>
+      <c r="L59" s="49">
+        <f t="shared" si="0"/>
+        <v>159.25943119496824</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="13">
       <c r="A60" s="43" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="24">
@@ -2310,15 +2426,22 @@
         <v>86.204819277108442</v>
       </c>
       <c r="I60" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K60" s="19">
+        <v>13910</v>
+      </c>
+      <c r="L60" s="49">
+        <f t="shared" si="0"/>
+        <v>16.254578161865052</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="13">
       <c r="A61" s="43" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="24">
@@ -2333,15 +2456,22 @@
         <v>21.820450281425892</v>
       </c>
       <c r="I61" s="40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K61" s="19">
+        <v>16390</v>
+      </c>
+      <c r="L61" s="49">
+        <f t="shared" si="0"/>
+        <v>174.43429591315598</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="13">
       <c r="A62" s="43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="24">
@@ -2356,15 +2486,22 @@
         <v>22.545391356905412</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K62" s="19">
+        <v>16980</v>
+      </c>
+      <c r="L62" s="49">
+        <f t="shared" si="0"/>
+        <v>117.51043745889932</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="13">
       <c r="A63" s="43" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="24">
@@ -2379,15 +2516,22 @@
         <v>49.094871794871793</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K63" s="19">
+        <v>9070</v>
+      </c>
+      <c r="L63" s="49">
+        <f t="shared" si="0"/>
+        <v>14.089941456621197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="13">
       <c r="A64" s="43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="24">
@@ -2402,15 +2546,22 @@
         <v>31.162500000000001</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="K64" s="19">
+        <v>22900</v>
+      </c>
+      <c r="L64" s="49">
+        <f t="shared" si="0"/>
+        <v>64.938421344371278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="13">
       <c r="A65" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="24">
@@ -2425,15 +2576,19 @@
         <v>0</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L65" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="13">
       <c r="A66" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="24">
@@ -2448,15 +2603,19 @@
         <v>0</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L66" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="13">
       <c r="A67" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="24">
@@ -2471,15 +2630,19 @@
         <v>0</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L67" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="13">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="24">
@@ -2494,10 +2657,14 @@
         <v>0</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="L68" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="13">
       <c r="A69" s="8" t="s">
         <v>31</v>
       </c>
@@ -2517,15 +2684,19 @@
         <v>0</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="L69" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="13">
       <c r="A70" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C70" s="51" t="s">
         <v>71</v>
@@ -2537,15 +2708,19 @@
         <v>72</v>
       </c>
       <c r="H70" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="L70" s="50">
+        <f>SUM(L43:L69)</f>
+        <v>4241.3995895572552</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="13">
       <c r="A71" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C71" s="24">
         <v>1</v>
@@ -2563,15 +2738,15 @@
         <v>40</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="13">
       <c r="A72" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C72" s="24">
         <v>0.75</v>
@@ -2589,15 +2764,15 @@
         <v>15</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="13">
       <c r="A73" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C73" s="24">
         <f>260/420</f>
@@ -2619,15 +2794,15 @@
         <v>100</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="13">
       <c r="A74" s="34" t="s">
         <v>36</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C74" s="24">
         <v>0.5</v>
@@ -2645,10 +2820,10 @@
         <v>100</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="13">
       <c r="A75" s="34" t="s">
         <v>37</v>
       </c>
@@ -2671,15 +2846,15 @@
         <v>0</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="13">
       <c r="A76" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C76" s="24">
         <v>1</v>
@@ -2697,10 +2872,10 @@
         <v>200</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="13">
       <c r="A77" s="34" t="s">
         <v>39</v>
       </c>
@@ -2723,15 +2898,15 @@
         <v>0</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="13">
       <c r="A78" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C78" s="24">
         <v>1</v>
@@ -2750,15 +2925,15 @@
         <v>300</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="13">
       <c r="A79" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C79" s="24">
         <v>1</v>
@@ -2778,15 +2953,15 @@
         <v>88</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="13">
       <c r="A80" s="34" t="s">
         <v>69</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="24">
         <v>1</v>
@@ -2804,10 +2979,10 @@
         <v>60</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="13">
       <c r="A81" s="34" t="s">
         <v>1</v>
       </c>
@@ -2830,15 +3005,15 @@
         <v>0</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="13">
       <c r="A82" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="24">
@@ -2850,12 +3025,12 @@
         <v>7.5</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="13">
       <c r="A83" s="32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B83" s="33"/>
       <c r="C83" s="51" t="s">
@@ -2868,15 +3043,15 @@
         <v>72</v>
       </c>
       <c r="H83" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="13">
       <c r="A84" s="34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C84" s="31"/>
       <c r="D84" s="24">
@@ -2892,15 +3067,15 @@
         <v>1</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="13">
       <c r="A85" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C85" s="31"/>
       <c r="D85" s="24">
@@ -2916,12 +3091,12 @@
         <v>1</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="13">
       <c r="A86" s="32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B86" s="33"/>
       <c r="C86" s="51" t="s">
@@ -2934,10 +3109,10 @@
         <v>72</v>
       </c>
       <c r="H86" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="13">
       <c r="A87" s="8" t="s">
         <v>70</v>
       </c>
@@ -2960,15 +3135,15 @@
         <v>0</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="13">
       <c r="A88" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C88" s="31"/>
       <c r="D88" s="24">
@@ -2980,10 +3155,10 @@
         <v>0</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="13">
       <c r="A89" s="32" t="s">
         <v>40</v>
       </c>
@@ -2998,15 +3173,15 @@
         <v>72</v>
       </c>
       <c r="H89" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="13">
       <c r="A90" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C90" s="31"/>
       <c r="D90" s="24">
@@ -3019,10 +3194,10 @@
         <v>16.666666666666668</v>
       </c>
       <c r="I90" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="13">
       <c r="A91" s="8" t="s">
         <v>42</v>
       </c>
@@ -3045,10 +3220,10 @@
         <v>0</v>
       </c>
       <c r="I91" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="13">
       <c r="A92" s="32" t="s">
         <v>43</v>
       </c>
@@ -3063,15 +3238,15 @@
         <v>72</v>
       </c>
       <c r="H92" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="13">
       <c r="A93" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C93" s="24">
         <v>1</v>
@@ -3092,15 +3267,15 @@
         <v>150</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="13">
       <c r="A94" s="34" t="s">
         <v>45</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C94" s="31"/>
       <c r="D94" s="24">
@@ -3112,10 +3287,10 @@
         <v>70</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="13">
       <c r="A95" s="32" t="s">
         <v>46</v>
       </c>
@@ -3130,10 +3305,10 @@
         <v>72</v>
       </c>
       <c r="H95" s="46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="13">
       <c r="A96" s="34" t="s">
         <v>47</v>
       </c>
@@ -3156,10 +3331,10 @@
         <v>0</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="13">
       <c r="A97" s="8" t="s">
         <v>48</v>
       </c>
@@ -3182,10 +3357,10 @@
         <v>0</v>
       </c>
       <c r="I97" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="13">
       <c r="A98" s="34" t="s">
         <v>49</v>
       </c>
@@ -3208,10 +3383,10 @@
         <v>0</v>
       </c>
       <c r="I98" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="13">
       <c r="A99" s="34" t="s">
         <v>50</v>
       </c>
@@ -3234,10 +3409,10 @@
         <v>0</v>
       </c>
       <c r="I99" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="13">
       <c r="A100" s="34" t="s">
         <v>51</v>
       </c>
@@ -3260,10 +3435,10 @@
         <v>0</v>
       </c>
       <c r="I100" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="13">
       <c r="A101" s="34" t="s">
         <v>52</v>
       </c>
@@ -3286,10 +3461,10 @@
         <v>0</v>
       </c>
       <c r="I101" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="13">
       <c r="A102" s="34" t="s">
         <v>53</v>
       </c>
@@ -3312,10 +3487,10 @@
         <v>0</v>
       </c>
       <c r="I102" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="13">
       <c r="A103" s="34" t="s">
         <v>54</v>
       </c>
@@ -3338,10 +3513,10 @@
         <v>0</v>
       </c>
       <c r="I103" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="13">
       <c r="A104" s="8" t="s">
         <v>55</v>
       </c>
@@ -3364,10 +3539,10 @@
         <v>0</v>
       </c>
       <c r="I104" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="13">
       <c r="A105" s="8" t="s">
         <v>56</v>
       </c>
@@ -3390,20 +3565,19 @@
         <v>0</v>
       </c>
       <c r="I105" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="G106" s="19"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9">
       <c r="G107" s="19"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9">
       <c r="G108" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="7">
     <mergeCell ref="C92:F92"/>
     <mergeCell ref="C95:F95"/>

</xml_diff>

<commit_message>
fixed zaloc & zalcm, expandability factors
</commit_message>
<xml_diff>
--- a/za_expandabilityfactors.xlsx
+++ b/za_expandabilityfactors.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="112">
   <si>
     <t>WEALTH GROUP</t>
   </si>
@@ -414,9 +414,6 @@
     <t>beef</t>
   </si>
   <si>
-    <t>dis</t>
-  </si>
-  <si>
     <t>ubpl</t>
   </si>
   <si>
@@ -441,7 +438,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -779,6 +776,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="72" applyFont="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,7 +786,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="75">
     <cellStyle name="Comma" xfId="72" builtinId="3"/>
@@ -1293,10 +1290,10 @@
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="L43" sqref="L43"/>
+      <selection pane="topRight" activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1323,7 +1320,7 @@
         <v>98</v>
       </c>
       <c r="E1" s="31"/>
-      <c r="F1" s="54">
+      <c r="F1" s="51">
         <v>4.1867999999999999</v>
       </c>
     </row>
@@ -1878,14 +1875,14 @@
         <v>28</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
       <c r="G42" s="46" t="s">
         <v>100</v>
       </c>
@@ -2684,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L69" s="49">
         <f t="shared" si="0"/>
@@ -2696,14 +2693,14 @@
         <v>32</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C70" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D70" s="52"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="54"/>
       <c r="G70" s="46" t="s">
         <v>72</v>
       </c>
@@ -3030,15 +3027,15 @@
     </row>
     <row r="83" spans="1:9" ht="13">
       <c r="A83" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B83" s="33"/>
-      <c r="C83" s="51" t="s">
+      <c r="C83" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D83" s="52"/>
-      <c r="E83" s="52"/>
-      <c r="F83" s="53"/>
+      <c r="D83" s="53"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="54"/>
       <c r="G83" s="46" t="s">
         <v>72</v>
       </c>
@@ -3048,7 +3045,7 @@
     </row>
     <row r="84" spans="1:9" ht="13">
       <c r="A84" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84" s="30" t="s">
         <v>99</v>
@@ -3072,7 +3069,7 @@
     </row>
     <row r="85" spans="1:9" ht="13">
       <c r="A85" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B85" s="30" t="s">
         <v>99</v>
@@ -3091,20 +3088,20 @@
         <v>1</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="13">
       <c r="A86" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="33"/>
-      <c r="C86" s="51" t="s">
+      <c r="C86" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D86" s="52"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="53"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="54"/>
       <c r="G86" s="46" t="s">
         <v>72</v>
       </c>
@@ -3155,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="13">
@@ -3163,12 +3160,12 @@
         <v>40</v>
       </c>
       <c r="B89" s="33"/>
-      <c r="C89" s="51" t="s">
+      <c r="C89" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D89" s="52"/>
-      <c r="E89" s="52"/>
-      <c r="F89" s="53"/>
+      <c r="D89" s="53"/>
+      <c r="E89" s="53"/>
+      <c r="F89" s="54"/>
       <c r="G89" s="46" t="s">
         <v>72</v>
       </c>
@@ -3228,12 +3225,12 @@
         <v>43</v>
       </c>
       <c r="B92" s="33"/>
-      <c r="C92" s="51" t="s">
+      <c r="C92" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D92" s="52"/>
-      <c r="E92" s="52"/>
-      <c r="F92" s="53"/>
+      <c r="D92" s="53"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="54"/>
       <c r="G92" s="46" t="s">
         <v>72</v>
       </c>
@@ -3295,12 +3292,12 @@
         <v>46</v>
       </c>
       <c r="B95" s="33"/>
-      <c r="C95" s="51" t="s">
+      <c r="C95" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D95" s="52"/>
-      <c r="E95" s="52"/>
-      <c r="F95" s="53"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="54"/>
       <c r="G95" s="46" t="s">
         <v>72</v>
       </c>

</xml_diff>